<commit_message>
Add logic for calculating total_paid for each insurance
</commit_message>
<xml_diff>
--- a/Records.xlsx
+++ b/Records.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Else\Creations\CashFlowApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Else\Creations\CashFlowApp\RiverOfGold\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C9B895-46F2-4B84-9F87-0FFAFEB3AF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0CBC90-7BAD-4F5D-8AE2-E71A8C170F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>一次支付</t>
   </si>
@@ -41,15 +41,6 @@
     <t>年金保险</t>
   </si>
   <si>
-    <t xml:space="preserve">支付金额 </t>
-  </si>
-  <si>
-    <t>付款周期（月）</t>
-  </si>
-  <si>
-    <t>付款持续时间（年）</t>
-  </si>
-  <si>
     <t>返还周期（月）</t>
   </si>
   <si>
@@ -80,12 +71,6 @@
     <t>保险单号</t>
   </si>
   <si>
-    <t>？年到期</t>
-  </si>
-  <si>
-    <t>返还升值比例（%）</t>
-  </si>
-  <si>
     <t>2013年7月15日开始扣款，每月1000元，扣十年。满20年，返已交保费的1.3倍</t>
   </si>
   <si>
@@ -102,13 +87,40 @@
   </si>
   <si>
     <t>日</t>
+  </si>
+  <si>
+    <t>都来保险</t>
+  </si>
+  <si>
+    <t>交费期间（年）</t>
+  </si>
+  <si>
+    <t>保险期间（年）</t>
+  </si>
+  <si>
+    <t>消费型</t>
+  </si>
+  <si>
+    <t>分期付满期返</t>
+  </si>
+  <si>
+    <t>意外险</t>
+  </si>
+  <si>
+    <t>返还比例（%）</t>
+  </si>
+  <si>
+    <t>支付金额</t>
+  </si>
+  <si>
+    <t>每年交费次数</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +132,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -145,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -162,6 +181,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,26 +463,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9135B11-7406-4FD9-8CD7-6BCD78398E28}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C16" sqref="C16"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36" style="10" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.453125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="11.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.54296875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="4" style="9" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.90625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.90625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.36328125" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.90625" style="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19" style="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.36328125" style="7" bestFit="1" customWidth="1"/>
@@ -469,54 +490,54 @@
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -539,15 +560,15 @@
         <v>2</v>
       </c>
       <c r="L2" s="5">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="O2" s="7">
-        <v>0.01</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -567,7 +588,7 @@
         <v>200</v>
       </c>
       <c r="I3" s="9">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J3" s="9">
         <v>1</v>
@@ -575,7 +596,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -595,7 +616,7 @@
         <v>10000</v>
       </c>
       <c r="I4" s="9">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J4" s="9">
         <v>5</v>
@@ -610,15 +631,15 @@
         <v>20</v>
       </c>
       <c r="O4" s="7">
-        <v>0.02</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E5" s="9">
         <v>2013</v>
@@ -633,7 +654,7 @@
         <v>1000</v>
       </c>
       <c r="I5" s="9">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J5" s="9">
         <v>10</v>
@@ -643,6 +664,67 @@
       </c>
       <c r="O5" s="7">
         <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2019</v>
+      </c>
+      <c r="F6" s="9">
+        <v>3</v>
+      </c>
+      <c r="G6" s="9">
+        <v>28</v>
+      </c>
+      <c r="H6" s="5">
+        <v>720</v>
+      </c>
+      <c r="I6" s="9">
+        <v>12</v>
+      </c>
+      <c r="J6" s="9">
+        <v>10</v>
+      </c>
+      <c r="K6" s="9">
+        <v>20</v>
+      </c>
+      <c r="L6" s="5">
+        <v>475200</v>
+      </c>
+      <c r="O6" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2020</v>
+      </c>
+      <c r="F7" s="9">
+        <v>6</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>397</v>
+      </c>
+      <c r="I7" s="9">
+        <v>12</v>
+      </c>
+      <c r="J7" s="9">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -663,10 +745,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>